<commit_message>
Add analysis files and update repository content
</commit_message>
<xml_diff>
--- a/Within_Viral_Species_Analyses/HPIV-2_p-distance.xlsx
+++ b/Within_Viral_Species_Analyses/HPIV-2_p-distance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greningerlab-macbook-2/Documents/HPIV/MANUSCRIPT/github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greningerlab-macbook-2/Documents/HPIV/HN_partial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721C55D0-0065-9844-97F6-4A293361F657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{88757ADB-C1F8-4045-ACC9-CE85A491DC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="880" windowWidth="28540" windowHeight="17340" xr2:uid="{669A8346-0C55-2442-8AEF-99E8D6A28F22}"/>
+    <workbookView xWindow="1380" yWindow="1020" windowWidth="28540" windowHeight="17340" xr2:uid="{669A8346-0C55-2442-8AEF-99E8D6A28F22}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix-p-distance" sheetId="1" r:id="rId1"/>
@@ -74,16 +74,16 @@
     <t>SE</t>
   </si>
   <si>
+    <t>The number of base differences per site from averaging over all sequence pairs within each group are shown. SE: standard error calculated by boostrap (100 replicates)</t>
+  </si>
+  <si>
+    <t>The number of base differences per site from averaging over all sequence pairs between groups are shown. SE: standard error calculated by boostrap (100 replicates)</t>
+  </si>
+  <si>
     <t>Table. Estimates of Evolutionary Divergence over Sequence Pairs between Groups with MEGAX</t>
   </si>
   <si>
     <t>Table. Estimates of Average Evolutionary Divergence over Sequence Pairs within Groups with MEGAX</t>
-  </si>
-  <si>
-    <t>The number of base differences per site (p-distance) from averaging over all sequence pairs between groups are shown. SE: standard error calculated by boostrap (100 replicates)</t>
-  </si>
-  <si>
-    <t>The number of base differences per site (p-distance)  from averaging over all sequence pairs within each group are shown. SE: standard error calculated by boostrap (100 replicates)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -592,12 +592,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -903,12 +903,12 @@
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>